<commit_message>
Adding update customer to SalesImport
</commit_message>
<xml_diff>
--- a/AppClasses/TestImport.xlsx
+++ b/AppClasses/TestImport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>Date</t>
   </si>
@@ -40,6 +40,12 @@
   </si>
   <si>
     <t>Marc@cs.com</t>
+  </si>
+  <si>
+    <t>Marc1@cs.com</t>
+  </si>
+  <si>
+    <t>Marc2@cs.com</t>
   </si>
 </sst>
 </file>
@@ -402,7 +408,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -472,7 +478,7 @@
         <v>5</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,7 +498,7 @@
         <v>20</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Bulk import for Products, Artists and Sales
</commit_message>
<xml_diff>
--- a/AppClasses/TestImport.xlsx
+++ b/AppClasses/TestImport.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Date</t>
   </si>
@@ -33,26 +33,14 @@
     <t>Item Discount (%)</t>
   </si>
   <si>
-    <t>Customer Email</t>
-  </si>
-  <si>
     <t>Marc</t>
-  </si>
-  <si>
-    <t>Marc@cs.com</t>
-  </si>
-  <si>
-    <t>Marc1@cs.com</t>
-  </si>
-  <si>
-    <t>Marc2@cs.com</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -65,14 +53,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -92,20 +72,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -405,10 +382,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F1" sqref="F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,10 +395,9 @@
     <col min="3" max="3" width="12.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -437,11 +413,8 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>40858</v>
       </c>
@@ -449,7 +422,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -457,19 +430,16 @@
       <c r="E2">
         <v>0</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>7</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>40859</v>
       </c>
       <c r="B3">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>5</v>
@@ -477,11 +447,8 @@
       <c r="E3">
         <v>5</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>8</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>40860</v>
       </c>
@@ -489,7 +456,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="D4">
         <v>6</v>
@@ -497,18 +464,11 @@
       <c r="E4">
         <v>20</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>9</v>
-      </c>
     </row>
+    <row r="16" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="F2" r:id="rId1"/>
-    <hyperlink ref="F3" r:id="rId2"/>
-    <hyperlink ref="F4" r:id="rId3"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Sales Management page addition
</commit_message>
<xml_diff>
--- a/AppClasses/TestImport.xlsx
+++ b/AppClasses/TestImport.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H11:H12"/>
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -442,13 +442,13 @@
         <v>40858</v>
       </c>
       <c r="B2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
       </c>
       <c r="D2">
-        <v>1</v>
+        <v>27</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -462,13 +462,13 @@
         <v>40859</v>
       </c>
       <c r="B3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C3" t="s">
         <v>5</v>
       </c>
       <c r="D3">
-        <v>5</v>
+        <v>28</v>
       </c>
       <c r="E3">
         <v>5</v>
@@ -482,13 +482,13 @@
         <v>40860</v>
       </c>
       <c r="B4">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
         <v>5</v>
       </c>
       <c r="D4">
-        <v>6</v>
+        <v>25</v>
       </c>
       <c r="E4">
         <v>20</v>

</xml_diff>